<commit_message>
update README and also add some dataset
</commit_message>
<xml_diff>
--- a/GeneratedTestData.xlsx
+++ b/GeneratedTestData.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmadar/Documents/capu/comp301/python-oner/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D2DCD8F0-F9F8-DA4C-8634-F99F7BC1B334}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F867082-7675-EE47-AB84-0131E37ACCA1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="16420" xr2:uid="{7629E89C-55EC-E546-AC3F-B427EC6DA70A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="approval" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -391,7 +391,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -417,33 +417,33 @@
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f ca="1">IF(RAND() &gt; 0.5, "Male", "Female")</f>
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="B2" t="str">
-        <f ca="1">IF(RAND()&gt;0.5, "LOW", "HIGH")</f>
+        <f ca="1">IF(RAND()&gt;0.6, "LOW", "HIGH")</f>
         <v>LOW</v>
       </c>
       <c r="C2" t="str">
-        <f ca="1">IF(RAND() &gt; 0.3, "Single",  "Married")</f>
-        <v>Single</v>
+        <f ca="1">IF(RAND() &gt; 0.6, "Single",  "Married")</f>
+        <v>Married</v>
       </c>
       <c r="D2" t="str">
         <f ca="1">IF(A2="Female",IF(RAND()&gt;0.2,"Yes","No"),IF(RAND()&gt;0.2,"No", "Yes"))</f>
-        <v>Yes</v>
+        <v>No</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A27" ca="1" si="0">IF(RAND() &gt; 0.5, "Male", "Female")</f>
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B27" ca="1" si="1">IF(RAND()&gt;0.5, "LOW", "HIGH")</f>
-        <v>LOW</v>
+        <f t="shared" ref="B3:B27" ca="1" si="1">IF(RAND()&gt;0.6, "LOW", "HIGH")</f>
+        <v>HIGH</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C27" ca="1" si="2">IF(RAND() &gt; 0.3, "Single",  "Married")</f>
-        <v>Single</v>
+        <f t="shared" ref="C3:C27" ca="1" si="2">IF(RAND() &gt; 0.6, "Single",  "Married")</f>
+        <v>Married</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D12" ca="1" si="3">IF(A3="Female",IF(RAND()&gt;0.2,"Yes","No"),IF(RAND()&gt;0.1,"No", "Yes"))</f>
@@ -453,7 +453,7 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -465,7 +465,7 @@
       </c>
       <c r="D4" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>No</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -475,11 +475,11 @@
       </c>
       <c r="B5" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LOW</v>
+        <v>HIGH</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Single</v>
+        <v>Married</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -501,7 +501,7 @@
       </c>
       <c r="D6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Yes</v>
+        <v>No</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -525,7 +525,7 @@
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -537,7 +537,7 @@
       </c>
       <c r="D8" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>No</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -551,7 +551,7 @@
       </c>
       <c r="C9" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Single</v>
+        <v>Married</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -565,7 +565,7 @@
       </c>
       <c r="B10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>HIGH</v>
+        <v>LOW</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -579,19 +579,19 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LOW</v>
+        <v>HIGH</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Single</v>
+        <v>Married</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>No</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -601,7 +601,7 @@
       </c>
       <c r="B12" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LOW</v>
+        <v>HIGH</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -609,13 +609,13 @@
       </c>
       <c r="D12" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>No</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -623,21 +623,21 @@
       </c>
       <c r="C13" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Married</v>
+        <v>Single</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" ref="D13:D27" ca="1" si="4">IF(A13="Female",IF(RAND()&gt;0.2,"Yes","No"),IF(RAND()&gt;0.1,"No", "Yes"))</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LOW</v>
+        <v>HIGH</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -651,11 +651,11 @@
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LOW</v>
+        <v>HIGH</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -663,7 +663,7 @@
       </c>
       <c r="D15" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Yes</v>
+        <v>No</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -691,11 +691,11 @@
       </c>
       <c r="B17" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LOW</v>
+        <v>HIGH</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Single</v>
+        <v>Married</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -705,7 +705,7 @@
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -713,11 +713,11 @@
       </c>
       <c r="C18" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Single</v>
+        <v>Married</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>No</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -727,7 +727,7 @@
       </c>
       <c r="B19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>HIGH</v>
+        <v>LOW</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -741,11 +741,11 @@
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="B20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>HIGH</v>
+        <v>LOW</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -753,13 +753,13 @@
       </c>
       <c r="D20" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>No</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Female</v>
+        <v>Male</v>
       </c>
       <c r="B21" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -799,7 +799,7 @@
       </c>
       <c r="B23" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>HIGH</v>
+        <v>LOW</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -807,17 +807,17 @@
       </c>
       <c r="D23" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>No</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="B24" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>HIGH</v>
+        <v>LOW</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -849,19 +849,19 @@
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Male</v>
+        <v>Female</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LOW</v>
+        <v>HIGH</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Single</v>
+        <v>Married</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>No</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -871,7 +871,7 @@
       </c>
       <c r="B27" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>HIGH</v>
+        <v>LOW</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" ca="1" si="2"/>

</xml_diff>